<commit_message>
update mvco-chl attribute defintiions
</commit_message>
<xml_diff>
--- a/nes-lter-chl-mvco-info.xlsx
+++ b/nes-lter-chl-mvco-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkoch\Desktop\LTER\nes-lter-chl-mvco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\nes-ims\nes-lter-chl-mvco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C15D13-B811-440D-B5C0-0B0097EEF2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C14383-2287-4594-99DC-B020292A4897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="1080" windowWidth="14400" windowHeight="8260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="116">
   <si>
     <t>attributeName</t>
   </si>
@@ -214,9 +214,6 @@
     <t>NOAA Large Marine Ecosystems</t>
   </si>
   <si>
-    <t>E. Taylor</t>
-  </si>
-  <si>
     <t>Crockford</t>
   </si>
   <si>
@@ -235,24 +232,15 @@
     <t>event_number</t>
   </si>
   <si>
-    <t>Identification number for each MVCO discrete sampling event</t>
-  </si>
-  <si>
     <t>event_number_niskin</t>
   </si>
   <si>
-    <t>Identification number for each Niskin or bucket collection during MVCO discrete sampling event</t>
-  </si>
-  <si>
     <t>ship</t>
   </si>
   <si>
     <t>Name of vessel from which samples were collected</t>
   </si>
   <si>
-    <t>Cruise identifer for the R/V Tioga</t>
-  </si>
-  <si>
     <t>Date and time in UTC when cast started or bucket filled</t>
   </si>
   <si>
@@ -374,13 +362,28 @@
   </si>
   <si>
     <t>cruise</t>
+  </si>
+  <si>
+    <t>Identification number for each sampling event, consisting of either MVCO event number or NES-LTER transect cruise and cast number</t>
+  </si>
+  <si>
+    <t>Identification number for each Niskin or bucket collection during MVCO discrete sampling event  or NES-LTER transect cruise, cast number, and Niskin number</t>
+  </si>
+  <si>
+    <t>Identifier for research cruise generally including abbreviation for research vessel and voyage number</t>
+  </si>
+  <si>
+    <t>E.</t>
+  </si>
+  <si>
+    <t>Taylor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +420,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -439,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -454,6 +463,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -735,20 +748,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="62.81640625" style="1" customWidth="1"/>
-    <col min="3" max="8" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" style="1" customWidth="1"/>
+    <col min="3" max="8" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -771,68 +784,68 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="G2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>110</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -841,18 +854,18 @@
         <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -861,18 +874,18 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -881,13 +894,13 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -901,107 +914,110 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1017,9 +1033,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1030,92 +1046,92 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
         <v>90</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
         <v>92</v>
-      </c>
-      <c r="C7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1128,15 +1144,15 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1168,7 +1184,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1200,7 +1216,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1232,18 +1248,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
         <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
         <v>44</v>
@@ -1258,18 +1277,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
         <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" t="s">
         <v>44</v>
@@ -1284,7 +1303,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1307,7 +1326,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1352,12 +1371,12 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1365,7 +1384,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -1373,84 +1392,84 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1466,9 +1485,9 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>

</xml_diff>